<commit_message>
Add code scraping hotmot site
</commit_message>
<xml_diff>
--- a/scraping_excel.xlsx
+++ b/scraping_excel.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\WorkSpace\1.ToDo\scrapingLunchMenu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\WorkSpace\1.ToDo\scrapingHotmotMenu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD455B8F-48C2-4CD8-A456-625BFF363A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A14173-DB42-4A26-8A86-5A958CCD8F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="甚兵衛" sheetId="1" r:id="rId1"/>
+    <sheet name="hotmot" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">甚兵衛!$A$1:$D$41</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">hotmot!$A$1:$D$41</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -349,15 +349,15 @@
   <dimension ref="A2:A48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:D1048576"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
   <cols>
     <col min="1" max="1" width="22.25" customWidth="1"/>
     <col min="2" max="2" width="23.125" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="20.875" customWidth="1"/>
+    <col min="3" max="3" width="22.25" customWidth="1"/>
+    <col min="4" max="4" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" ht="87.75" customHeight="1"/>

</xml_diff>